<commit_message>
serial interface updated in flash_bootloader_stm32f1x repo
</commit_message>
<xml_diff>
--- a/doc/Memorymap.xlsx
+++ b/doc/Memorymap.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CB Learning\Bootloader\git\bootmanager_stm32f1x\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAHESH\Desktop\STM32_Project\Bootloader_V1\flash_bootloader_stm32f1x-\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>08000000H</t>
   </si>
@@ -170,6 +170,18 @@
   </si>
   <si>
     <t>Size of kB</t>
+  </si>
+  <si>
+    <t>08001C00H</t>
+  </si>
+  <si>
+    <t>08005C00H</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>START</t>
   </si>
 </sst>
 </file>
@@ -379,6 +391,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -453,15 +474,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -745,61 +757,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="9" max="9" width="6.44140625" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
-    <col min="15" max="15" width="16.109375" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C3" s="5" t="s">
+    <row r="3" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="K3" s="24" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="Q3" s="13" t="s">
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="Q3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-    </row>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="J4" s="30" t="s">
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="17"/>
+    </row>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+      <c r="J4" s="5" t="s">
         <v>24</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-    </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
@@ -810,23 +828,23 @@
       <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="7">
         <v>7</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-    </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
@@ -837,19 +855,19 @@
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="31"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-    </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J6" s="7"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
@@ -860,38 +878,38 @@
       <c r="F7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-    </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C8" s="7" t="s">
+      <c r="J7" s="7"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-    </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
@@ -902,321 +920,330 @@
       <c r="F9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-    </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J9" s="7"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-    </row>
-    <row r="11" spans="3:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="6" t="s">
+      <c r="J10" s="7"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+    </row>
+    <row r="11" spans="3:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="J11" s="31">
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="I11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="7">
         <v>16</v>
       </c>
-      <c r="K11" s="25" t="s">
+      <c r="K11" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-    </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-    </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-    </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J14" s="31"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-    </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C15" s="29" t="s">
+      <c r="J13" s="7"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="J14" s="7"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C15" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-    </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C16" s="13" t="s">
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C16" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-    </row>
-    <row r="17" spans="3:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="J17" s="31">
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="V16" s="17"/>
+    </row>
+    <row r="17" spans="3:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="I17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="7">
         <v>104</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="K17" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="17" t="s">
+      <c r="L17" s="19"/>
+      <c r="M17" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="N17" s="18"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
-    </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="20"/>
+      <c r="N17" s="21"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="23"/>
       <c r="O18" s="4"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-    </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="19"/>
-      <c r="N19" s="20"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="23"/>
       <c r="O19" s="4"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-    </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="20"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="23"/>
       <c r="O20" s="4"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
-    </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="J21" s="31"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="19"/>
-      <c r="N21" s="20"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="23"/>
       <c r="O21" s="4"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
-    </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="20"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="23"/>
       <c r="O22" s="4"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="14"/>
-      <c r="V22" s="14"/>
-    </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J23" s="31"/>
-      <c r="K23" s="21" t="s">
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="J23" s="7"/>
+      <c r="K23" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="23"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="14"/>
-      <c r="V23" s="14"/>
-    </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J24" s="31">
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="26"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+    </row>
+    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="I24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" s="7">
         <v>1</v>
       </c>
-      <c r="K24" s="27" t="s">
+      <c r="K24" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
       <c r="O24" t="s">
         <v>6</v>
       </c>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
-      <c r="V24" s="14"/>
-    </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J25" s="31"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+    </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="7"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
       <c r="O25" t="s">
         <v>7</v>
       </c>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
-      <c r="V25" s="14"/>
-    </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="J26" s="32">
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="J26" s="6">
         <f>SUM(J5:J25)</f>
         <v>128</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="J17:J23"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C11:F12"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C4:F4"/>
     <mergeCell ref="Q3:V25"/>
     <mergeCell ref="K17:L22"/>
     <mergeCell ref="M17:N22"/>
@@ -1225,6 +1252,12 @@
     <mergeCell ref="K5:N10"/>
     <mergeCell ref="K11:N16"/>
     <mergeCell ref="K24:N25"/>
+    <mergeCell ref="J17:J23"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C11:F12"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C4:F4"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C16:F22"/>
     <mergeCell ref="J5:J10"/>

</xml_diff>

<commit_message>
Bootloader command and GNC GCC compilation doc files added and updated
</commit_message>
<xml_diff>
--- a/doc/Memorymap.xlsx
+++ b/doc/Memorymap.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAHESH\Desktop\STM32_Project\Bootloader_V1\flash_bootloader_stm32f1x-\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CB Learning\Bootloader\git\bootmanager_stm32f1x\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>08000000H</t>
   </si>
@@ -170,18 +170,6 @@
   </si>
   <si>
     <t>Size of kB</t>
-  </si>
-  <si>
-    <t>08001C00H</t>
-  </si>
-  <si>
-    <t>08005C00H</t>
-  </si>
-  <si>
-    <t>END</t>
-  </si>
-  <si>
-    <t>START</t>
   </si>
 </sst>
 </file>
@@ -391,89 +379,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,67 +745,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="15" max="15" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C3" s="8" t="s">
+    <row r="3" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="27" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="K3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="Q3" s="16" t="s">
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="Q3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-    </row>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-      <c r="J4" s="5" t="s">
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+    </row>
+    <row r="4" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="J4" s="30" t="s">
         <v>24</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
-    </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+    </row>
+    <row r="5" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
@@ -828,23 +810,23 @@
       <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="31">
         <v>7</v>
       </c>
-      <c r="K5" s="28" t="s">
+      <c r="K5" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="29"/>
-      <c r="M5" s="29"/>
-      <c r="N5" s="29"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-    </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+    </row>
+    <row r="6" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
@@ -855,19 +837,19 @@
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J6" s="7"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-    </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="J6" s="31"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+    </row>
+    <row r="7" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
@@ -878,38 +860,38 @@
       <c r="F7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="7"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="17"/>
-    </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C8" s="10" t="s">
+      <c r="J7" s="31"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-    </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
@@ -920,330 +902,321 @@
       <c r="F9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="17"/>
-      <c r="S9" s="17"/>
-      <c r="T9" s="17"/>
-      <c r="U9" s="17"/>
-      <c r="V9" s="17"/>
-    </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="J9" s="31"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
-      <c r="Q10" s="17"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17"/>
-    </row>
-    <row r="11" spans="3:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="9" t="s">
+      <c r="J10" s="31"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+    </row>
+    <row r="11" spans="3:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="I11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="7">
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="J11" s="31">
         <v>16</v>
       </c>
-      <c r="K11" s="28" t="s">
+      <c r="K11" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-    </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="17"/>
-      <c r="U12" s="17"/>
-      <c r="V12" s="17"/>
-    </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+    </row>
+    <row r="13" spans="3:22" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="17"/>
-      <c r="T13" s="17"/>
-      <c r="U13" s="17"/>
-      <c r="V13" s="17"/>
-    </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="J14" s="7"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="17"/>
-    </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C15" s="32" t="s">
+      <c r="J13" s="31"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+    </row>
+    <row r="14" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J14" s="31"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C15" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="17"/>
-      <c r="U15" s="17"/>
-      <c r="V15" s="17"/>
-    </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C16" s="16" t="s">
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C16" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="17"/>
-      <c r="S16" s="17"/>
-      <c r="T16" s="17"/>
-      <c r="U16" s="17"/>
-      <c r="V16" s="17"/>
-    </row>
-    <row r="17" spans="3:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="I17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="7">
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+    </row>
+    <row r="17" spans="3:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="J17" s="31">
         <v>104</v>
       </c>
-      <c r="K17" s="18" t="s">
+      <c r="K17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="20" t="s">
+      <c r="L17" s="16"/>
+      <c r="M17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="N17" s="21"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="17"/>
-      <c r="V17" s="17"/>
-    </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="23"/>
+      <c r="N17" s="18"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
+      <c r="V17" s="14"/>
+    </row>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="20"/>
       <c r="O18" s="4"/>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="17"/>
-      <c r="V18" s="17"/>
-    </row>
-    <row r="19" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="23"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+    </row>
+    <row r="19" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="20"/>
       <c r="O19" s="4"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
-      <c r="U19" s="17"/>
-      <c r="V19" s="17"/>
-    </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="23"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="14"/>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="20"/>
       <c r="O20" s="4"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="17"/>
-      <c r="S20" s="17"/>
-      <c r="T20" s="17"/>
-      <c r="U20" s="17"/>
-      <c r="V20" s="17"/>
-    </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="23"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="20"/>
       <c r="O21" s="4"/>
-      <c r="Q21" s="17"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17"/>
-      <c r="U21" s="17"/>
-      <c r="V21" s="17"/>
-    </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="23"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
+      <c r="V21" s="14"/>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="J22" s="31"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="20"/>
       <c r="O22" s="4"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
-      <c r="U22" s="17"/>
-      <c r="V22" s="17"/>
-    </row>
-    <row r="23" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="J23" s="7"/>
-      <c r="K23" s="24" t="s">
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="14"/>
+      <c r="V22" s="14"/>
+    </row>
+    <row r="23" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J23" s="31"/>
+      <c r="K23" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="26"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
-      <c r="U23" s="17"/>
-      <c r="V23" s="17"/>
-    </row>
-    <row r="24" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="I24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J24" s="7">
+      <c r="L23" s="22"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="23"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="14"/>
+    </row>
+    <row r="24" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J24" s="31">
         <v>1</v>
       </c>
-      <c r="K24" s="30" t="s">
+      <c r="K24" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
       <c r="O24" t="s">
         <v>6</v>
       </c>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
-      <c r="U24" s="17"/>
-      <c r="V24" s="17"/>
-    </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="H25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J25" s="7"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+      <c r="V24" s="14"/>
+    </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J25" s="31"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
       <c r="O25" t="s">
         <v>7</v>
       </c>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
-      <c r="U25" s="17"/>
-      <c r="V25" s="17"/>
-    </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="J26" s="6">
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="14"/>
+      <c r="U25" s="14"/>
+      <c r="V25" s="14"/>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="J26" s="32">
         <f>SUM(J5:J25)</f>
         <v>128</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="J17:J23"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C11:F12"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C4:F4"/>
     <mergeCell ref="Q3:V25"/>
     <mergeCell ref="K17:L22"/>
     <mergeCell ref="M17:N22"/>
@@ -1252,12 +1225,6 @@
     <mergeCell ref="K5:N10"/>
     <mergeCell ref="K11:N16"/>
     <mergeCell ref="K24:N25"/>
-    <mergeCell ref="J17:J23"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C11:F12"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C4:F4"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C16:F22"/>
     <mergeCell ref="J5:J10"/>

</xml_diff>